<commit_message>
23-07-25 Update expenditure and client Excel files
Revised 'Expenditure Mian Anjum Saeed.xlsx' in the Cash Book and 'Murtaza Lace.xlsx' in the Clients directory. Changes likely include updated financial or client data.
</commit_message>
<xml_diff>
--- a/Cash Book/Expenditure Mian Anjum Saeed.xlsx
+++ b/Cash Book/Expenditure Mian Anjum Saeed.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mian-Industries\Cash Book\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mian-Industries\Cash Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12429AC-1F20-4C77-8CCA-1D3CDD41AC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Up untill 2025" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="zt5VEtdFQn/DbdUmDWlfVAnffxhstJbwJwC9e/aXKFI="/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
   <si>
     <t>Date</t>
   </si>
@@ -147,19 +146,31 @@
     <t>Baraf</t>
   </si>
   <si>
-    <t>Needles</t>
-  </si>
-  <si>
     <t>miscellaneous</t>
   </si>
   <si>
-    <t>Petrol</t>
+    <t>AA bobbin 5 Boxes</t>
+  </si>
+  <si>
+    <t>Needles purchased from Tariq</t>
+  </si>
+  <si>
+    <t>From Arshad sb</t>
+  </si>
+  <si>
+    <t>Mian Arshad</t>
+  </si>
+  <si>
+    <t>Murtaza</t>
+  </si>
+  <si>
+    <t>Hussain lace payment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
@@ -462,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -522,6 +533,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -540,7 +552,8 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,20 +768,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" customHeight="1">
@@ -790,32 +803,41 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="26"/>
       <c r="K1" s="6">
         <f>D93</f>
-        <v>226230</v>
+        <v>293330</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1">
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
+      <c r="A2" s="11">
+        <v>45854</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="D2" s="8"/>
-      <c r="E2" s="4"/>
+      <c r="E2" s="4">
+        <v>250000</v>
+      </c>
       <c r="F2" s="9">
         <v>250000</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="27"/>
-      <c r="J2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
       <c r="K2" s="10">
         <f>F95</f>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1">
@@ -1297,8 +1319,8 @@
       <c r="A28" s="16">
         <v>45860</v>
       </c>
-      <c r="B28" s="33" t="s">
-        <v>40</v>
+      <c r="B28" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>23</v>
@@ -1316,7 +1338,7 @@
       <c r="A29" s="16">
         <v>45860</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -1335,8 +1357,8 @@
       <c r="A30" s="16">
         <v>45860</v>
       </c>
-      <c r="B30" s="33" t="s">
-        <v>41</v>
+      <c r="B30" s="23" t="s">
+        <v>40</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>23</v>
@@ -1354,41 +1376,49 @@
       <c r="A31" s="16">
         <v>45861</v>
       </c>
-      <c r="B31" s="33" t="s">
-        <v>42</v>
+      <c r="B31" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="D31" s="13">
-        <v>400</v>
+        <v>67500</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>-43330</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A32" s="16"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
+      <c r="A32" s="11">
+        <v>45855</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>45</v>
+      </c>
       <c r="D32" s="13"/>
-      <c r="E32" s="14"/>
+      <c r="E32" s="14">
+        <v>500000</v>
+      </c>
       <c r="F32" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A33" s="16"/>
-      <c r="B33" s="15"/>
+      <c r="A33" s="11"/>
+      <c r="B33" s="35"/>
       <c r="C33" s="15"/>
       <c r="D33" s="13"/>
       <c r="E33" s="14"/>
       <c r="F33" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.25" customHeight="1">
@@ -1399,7 +1429,7 @@
       <c r="E34" s="14"/>
       <c r="F34" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.25" customHeight="1">
@@ -1410,7 +1440,7 @@
       <c r="E35" s="14"/>
       <c r="F35" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.25" customHeight="1">
@@ -1421,7 +1451,7 @@
       <c r="E36" s="14"/>
       <c r="F36" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14.25" customHeight="1">
@@ -1432,7 +1462,7 @@
       <c r="E37" s="14"/>
       <c r="F37" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.25" customHeight="1">
@@ -1443,7 +1473,7 @@
       <c r="E38" s="14"/>
       <c r="F38" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="14.25" customHeight="1">
@@ -1454,7 +1484,7 @@
       <c r="E39" s="14"/>
       <c r="F39" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.25" customHeight="1">
@@ -1465,7 +1495,7 @@
       <c r="E40" s="14"/>
       <c r="F40" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.25" customHeight="1">
@@ -1476,7 +1506,7 @@
       <c r="E41" s="14"/>
       <c r="F41" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.25" customHeight="1">
@@ -1487,7 +1517,7 @@
       <c r="E42" s="14"/>
       <c r="F42" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.25" customHeight="1">
@@ -1498,7 +1528,7 @@
       <c r="E43" s="14"/>
       <c r="F43" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.25" customHeight="1">
@@ -1509,7 +1539,7 @@
       <c r="E44" s="14"/>
       <c r="F44" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.25" customHeight="1">
@@ -1520,7 +1550,7 @@
       <c r="E45" s="14"/>
       <c r="F45" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.25" customHeight="1">
@@ -1531,7 +1561,7 @@
       <c r="E46" s="14"/>
       <c r="F46" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="14.25" customHeight="1">
@@ -1542,7 +1572,7 @@
       <c r="E47" s="14"/>
       <c r="F47" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="14.25" customHeight="1">
@@ -1553,7 +1583,7 @@
       <c r="E48" s="14"/>
       <c r="F48" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="14.25" customHeight="1">
@@ -1564,7 +1594,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="14.25" customHeight="1">
@@ -1575,7 +1605,7 @@
       <c r="E50" s="14"/>
       <c r="F50" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="14.25" customHeight="1">
@@ -1586,7 +1616,7 @@
       <c r="E51" s="14"/>
       <c r="F51" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="14.25" customHeight="1">
@@ -1597,7 +1627,7 @@
       <c r="E52" s="14"/>
       <c r="F52" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.25" customHeight="1">
@@ -1608,7 +1638,7 @@
       <c r="E53" s="14"/>
       <c r="F53" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="14.25" customHeight="1">
@@ -1619,7 +1649,7 @@
       <c r="E54" s="14"/>
       <c r="F54" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="14.25" customHeight="1">
@@ -1630,7 +1660,7 @@
       <c r="E55" s="14"/>
       <c r="F55" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="14.25" customHeight="1">
@@ -1641,7 +1671,7 @@
       <c r="E56" s="14"/>
       <c r="F56" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="14.25" customHeight="1">
@@ -1652,7 +1682,7 @@
       <c r="E57" s="14"/>
       <c r="F57" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="14.25" customHeight="1">
@@ -1663,7 +1693,7 @@
       <c r="E58" s="14"/>
       <c r="F58" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="14.25" customHeight="1">
@@ -1674,7 +1704,7 @@
       <c r="E59" s="14"/>
       <c r="F59" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="14.25" customHeight="1">
@@ -1685,7 +1715,7 @@
       <c r="E60" s="14"/>
       <c r="F60" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="14.25" customHeight="1">
@@ -1696,7 +1726,7 @@
       <c r="E61" s="14"/>
       <c r="F61" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="14.25" customHeight="1">
@@ -1707,7 +1737,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="14.25" customHeight="1">
@@ -1718,7 +1748,7 @@
       <c r="E63" s="14"/>
       <c r="F63" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="14.25" customHeight="1">
@@ -1729,7 +1759,7 @@
       <c r="E64" s="14"/>
       <c r="F64" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="14.25" customHeight="1">
@@ -1740,7 +1770,7 @@
       <c r="E65" s="14"/>
       <c r="F65" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="14.25" customHeight="1">
@@ -1751,7 +1781,7 @@
       <c r="E66" s="14"/>
       <c r="F66" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="14.25" customHeight="1">
@@ -1762,7 +1792,7 @@
       <c r="E67" s="14"/>
       <c r="F67" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="14.25" customHeight="1">
@@ -1773,7 +1803,7 @@
       <c r="E68" s="14"/>
       <c r="F68" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="14.25" customHeight="1">
@@ -1784,7 +1814,7 @@
       <c r="E69" s="14"/>
       <c r="F69" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="14.25" customHeight="1">
@@ -1795,7 +1825,7 @@
       <c r="E70" s="14"/>
       <c r="F70" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="14.25" customHeight="1">
@@ -1806,7 +1836,7 @@
       <c r="E71" s="14"/>
       <c r="F71" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="14.25" customHeight="1">
@@ -1817,7 +1847,7 @@
       <c r="E72" s="14"/>
       <c r="F72" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="14.25" customHeight="1">
@@ -1828,7 +1858,7 @@
       <c r="E73" s="14"/>
       <c r="F73" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="14.25" customHeight="1">
@@ -1839,7 +1869,7 @@
       <c r="E74" s="14"/>
       <c r="F74" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="14.25" customHeight="1">
@@ -1850,7 +1880,7 @@
       <c r="E75" s="14"/>
       <c r="F75" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="14.25" customHeight="1">
@@ -1861,7 +1891,7 @@
       <c r="E76" s="14"/>
       <c r="F76" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="14.25" customHeight="1">
@@ -1872,7 +1902,7 @@
       <c r="E77" s="14"/>
       <c r="F77" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="14.25" customHeight="1">
@@ -1883,7 +1913,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="14.25" customHeight="1">
@@ -1894,7 +1924,7 @@
       <c r="E79" s="14"/>
       <c r="F79" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="14.25" customHeight="1">
@@ -1905,7 +1935,7 @@
       <c r="E80" s="14"/>
       <c r="F80" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="14.25" customHeight="1">
@@ -1916,7 +1946,7 @@
       <c r="E81" s="14"/>
       <c r="F81" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="14.25" customHeight="1">
@@ -1927,7 +1957,7 @@
       <c r="E82" s="14"/>
       <c r="F82" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="14.25" customHeight="1">
@@ -1938,7 +1968,7 @@
       <c r="E83" s="14"/>
       <c r="F83" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="14.25" customHeight="1">
@@ -1949,7 +1979,7 @@
       <c r="E84" s="14"/>
       <c r="F84" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="14.25" customHeight="1">
@@ -1960,7 +1990,7 @@
       <c r="E85" s="14"/>
       <c r="F85" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="14.25" customHeight="1">
@@ -1971,7 +2001,7 @@
       <c r="E86" s="14"/>
       <c r="F86" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="14.25" customHeight="1">
@@ -1982,7 +2012,7 @@
       <c r="E87" s="14"/>
       <c r="F87" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="14.25" customHeight="1">
@@ -1992,7 +2022,7 @@
       <c r="E88" s="14"/>
       <c r="F88" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="14.25" customHeight="1">
@@ -2003,7 +2033,7 @@
       <c r="E89" s="14"/>
       <c r="F89" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="14.25" customHeight="1">
@@ -2014,7 +2044,7 @@
       <c r="E90" s="14"/>
       <c r="F90" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="14.25" customHeight="1">
@@ -2025,7 +2055,7 @@
       <c r="E91" s="14"/>
       <c r="F91" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="14.25" customHeight="1">
@@ -2036,52 +2066,52 @@
       <c r="E92" s="14"/>
       <c r="F92" s="9">
         <f t="shared" si="0"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A93" s="23" t="s">
+      <c r="A93" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="24"/>
-      <c r="C93" s="25"/>
+      <c r="B93" s="25"/>
+      <c r="C93" s="26"/>
       <c r="D93" s="6">
         <f>SUM(D3:D92)</f>
-        <v>226230</v>
+        <v>293330</v>
       </c>
       <c r="E93" s="17"/>
       <c r="F93" s="9">
         <f t="shared" ref="F93:F94" si="1">F91</f>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A94" s="29" t="s">
+      <c r="A94" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B94" s="27"/>
-      <c r="C94" s="27"/>
-      <c r="D94" s="28"/>
+      <c r="B94" s="28"/>
+      <c r="C94" s="28"/>
+      <c r="D94" s="29"/>
       <c r="E94" s="18">
         <f>SUM(E11:E92)</f>
-        <v>0</v>
+        <v>500000</v>
       </c>
       <c r="F94" s="9">
         <f t="shared" si="1"/>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A95" s="30" t="s">
+      <c r="A95" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="B95" s="31"/>
-      <c r="C95" s="31"/>
-      <c r="D95" s="31"/>
-      <c r="E95" s="32"/>
+      <c r="B95" s="32"/>
+      <c r="C95" s="32"/>
+      <c r="D95" s="32"/>
+      <c r="E95" s="33"/>
       <c r="F95" s="19">
         <f>F92</f>
-        <v>23770</v>
+        <v>456670</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
23--07-25 Update expenditure spreadsheet for Mian Anjum Saeed
Revised the 'Expenditure Mian Anjum Saeed.xlsx' file with updated data or corrections.
</commit_message>
<xml_diff>
--- a/Cash Book/Expenditure Mian Anjum Saeed.xlsx
+++ b/Cash Book/Expenditure Mian Anjum Saeed.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="48">
   <si>
     <t>Date</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Hussain lace payment</t>
+  </si>
+  <si>
+    <t>Cash payment to Shabaz</t>
   </si>
 </sst>
 </file>
@@ -534,6 +537,8 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -552,8 +557,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -803,14 +806,14 @@
       <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="25"/>
-      <c r="J1" s="26"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="6">
         <f>D93</f>
-        <v>293330</v>
+        <v>643330</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.25" customHeight="1">
@@ -830,14 +833,14 @@
       <c r="F2" s="9">
         <v>250000</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="28"/>
-      <c r="J2" s="29"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="31"/>
       <c r="K2" s="10">
         <f>F95</f>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.25" customHeight="1">
@@ -1395,7 +1398,7 @@
       <c r="A32" s="11">
         <v>45855</v>
       </c>
-      <c r="B32" s="34" t="s">
+      <c r="B32" s="24" t="s">
         <v>46</v>
       </c>
       <c r="C32" s="15" t="s">
@@ -1411,14 +1414,22 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="35"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="13"/>
+      <c r="A33" s="11">
+        <v>45859</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" s="13">
+        <v>350000</v>
+      </c>
       <c r="E33" s="14"/>
       <c r="F33" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="14.25" customHeight="1">
@@ -1429,7 +1440,7 @@
       <c r="E34" s="14"/>
       <c r="F34" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="14.25" customHeight="1">
@@ -1440,7 +1451,7 @@
       <c r="E35" s="14"/>
       <c r="F35" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="14.25" customHeight="1">
@@ -1451,7 +1462,7 @@
       <c r="E36" s="14"/>
       <c r="F36" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="14.25" customHeight="1">
@@ -1462,7 +1473,7 @@
       <c r="E37" s="14"/>
       <c r="F37" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="14.25" customHeight="1">
@@ -1473,7 +1484,7 @@
       <c r="E38" s="14"/>
       <c r="F38" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="14.25" customHeight="1">
@@ -1484,7 +1495,7 @@
       <c r="E39" s="14"/>
       <c r="F39" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="14.25" customHeight="1">
@@ -1495,7 +1506,7 @@
       <c r="E40" s="14"/>
       <c r="F40" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="14.25" customHeight="1">
@@ -1506,7 +1517,7 @@
       <c r="E41" s="14"/>
       <c r="F41" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="14.25" customHeight="1">
@@ -1517,7 +1528,7 @@
       <c r="E42" s="14"/>
       <c r="F42" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="14.25" customHeight="1">
@@ -1528,7 +1539,7 @@
       <c r="E43" s="14"/>
       <c r="F43" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="14.25" customHeight="1">
@@ -1539,7 +1550,7 @@
       <c r="E44" s="14"/>
       <c r="F44" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="14.25" customHeight="1">
@@ -1550,7 +1561,7 @@
       <c r="E45" s="14"/>
       <c r="F45" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="14.25" customHeight="1">
@@ -1561,7 +1572,7 @@
       <c r="E46" s="14"/>
       <c r="F46" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="14.25" customHeight="1">
@@ -1572,7 +1583,7 @@
       <c r="E47" s="14"/>
       <c r="F47" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="14.25" customHeight="1">
@@ -1583,7 +1594,7 @@
       <c r="E48" s="14"/>
       <c r="F48" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="14.25" customHeight="1">
@@ -1594,7 +1605,7 @@
       <c r="E49" s="14"/>
       <c r="F49" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="14.25" customHeight="1">
@@ -1605,7 +1616,7 @@
       <c r="E50" s="14"/>
       <c r="F50" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="14.25" customHeight="1">
@@ -1616,7 +1627,7 @@
       <c r="E51" s="14"/>
       <c r="F51" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="14.25" customHeight="1">
@@ -1627,7 +1638,7 @@
       <c r="E52" s="14"/>
       <c r="F52" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="14.25" customHeight="1">
@@ -1638,7 +1649,7 @@
       <c r="E53" s="14"/>
       <c r="F53" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="14.25" customHeight="1">
@@ -1649,7 +1660,7 @@
       <c r="E54" s="14"/>
       <c r="F54" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="14.25" customHeight="1">
@@ -1660,7 +1671,7 @@
       <c r="E55" s="14"/>
       <c r="F55" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="14.25" customHeight="1">
@@ -1671,7 +1682,7 @@
       <c r="E56" s="14"/>
       <c r="F56" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="14.25" customHeight="1">
@@ -1682,7 +1693,7 @@
       <c r="E57" s="14"/>
       <c r="F57" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="14.25" customHeight="1">
@@ -1693,7 +1704,7 @@
       <c r="E58" s="14"/>
       <c r="F58" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="14.25" customHeight="1">
@@ -1704,7 +1715,7 @@
       <c r="E59" s="14"/>
       <c r="F59" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="14.25" customHeight="1">
@@ -1715,7 +1726,7 @@
       <c r="E60" s="14"/>
       <c r="F60" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="14.25" customHeight="1">
@@ -1726,7 +1737,7 @@
       <c r="E61" s="14"/>
       <c r="F61" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="14.25" customHeight="1">
@@ -1737,7 +1748,7 @@
       <c r="E62" s="14"/>
       <c r="F62" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="14.25" customHeight="1">
@@ -1748,7 +1759,7 @@
       <c r="E63" s="14"/>
       <c r="F63" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="14.25" customHeight="1">
@@ -1759,7 +1770,7 @@
       <c r="E64" s="14"/>
       <c r="F64" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="65" spans="1:6" ht="14.25" customHeight="1">
@@ -1770,7 +1781,7 @@
       <c r="E65" s="14"/>
       <c r="F65" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="66" spans="1:6" ht="14.25" customHeight="1">
@@ -1781,7 +1792,7 @@
       <c r="E66" s="14"/>
       <c r="F66" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="14.25" customHeight="1">
@@ -1792,7 +1803,7 @@
       <c r="E67" s="14"/>
       <c r="F67" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="68" spans="1:6" ht="14.25" customHeight="1">
@@ -1803,7 +1814,7 @@
       <c r="E68" s="14"/>
       <c r="F68" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="69" spans="1:6" ht="14.25" customHeight="1">
@@ -1814,7 +1825,7 @@
       <c r="E69" s="14"/>
       <c r="F69" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="14.25" customHeight="1">
@@ -1825,7 +1836,7 @@
       <c r="E70" s="14"/>
       <c r="F70" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="14.25" customHeight="1">
@@ -1836,7 +1847,7 @@
       <c r="E71" s="14"/>
       <c r="F71" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="72" spans="1:6" ht="14.25" customHeight="1">
@@ -1847,7 +1858,7 @@
       <c r="E72" s="14"/>
       <c r="F72" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="73" spans="1:6" ht="14.25" customHeight="1">
@@ -1858,7 +1869,7 @@
       <c r="E73" s="14"/>
       <c r="F73" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="74" spans="1:6" ht="14.25" customHeight="1">
@@ -1869,7 +1880,7 @@
       <c r="E74" s="14"/>
       <c r="F74" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="75" spans="1:6" ht="14.25" customHeight="1">
@@ -1880,7 +1891,7 @@
       <c r="E75" s="14"/>
       <c r="F75" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="76" spans="1:6" ht="14.25" customHeight="1">
@@ -1891,7 +1902,7 @@
       <c r="E76" s="14"/>
       <c r="F76" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="77" spans="1:6" ht="14.25" customHeight="1">
@@ -1902,7 +1913,7 @@
       <c r="E77" s="14"/>
       <c r="F77" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="78" spans="1:6" ht="14.25" customHeight="1">
@@ -1913,7 +1924,7 @@
       <c r="E78" s="14"/>
       <c r="F78" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="79" spans="1:6" ht="14.25" customHeight="1">
@@ -1924,7 +1935,7 @@
       <c r="E79" s="14"/>
       <c r="F79" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="14.25" customHeight="1">
@@ -1935,7 +1946,7 @@
       <c r="E80" s="14"/>
       <c r="F80" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="81" spans="1:6" ht="14.25" customHeight="1">
@@ -1946,7 +1957,7 @@
       <c r="E81" s="14"/>
       <c r="F81" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="82" spans="1:6" ht="14.25" customHeight="1">
@@ -1957,7 +1968,7 @@
       <c r="E82" s="14"/>
       <c r="F82" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="83" spans="1:6" ht="14.25" customHeight="1">
@@ -1968,7 +1979,7 @@
       <c r="E83" s="14"/>
       <c r="F83" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="84" spans="1:6" ht="14.25" customHeight="1">
@@ -1979,7 +1990,7 @@
       <c r="E84" s="14"/>
       <c r="F84" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="85" spans="1:6" ht="14.25" customHeight="1">
@@ -1990,7 +2001,7 @@
       <c r="E85" s="14"/>
       <c r="F85" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="86" spans="1:6" ht="14.25" customHeight="1">
@@ -2001,7 +2012,7 @@
       <c r="E86" s="14"/>
       <c r="F86" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="87" spans="1:6" ht="14.25" customHeight="1">
@@ -2012,7 +2023,7 @@
       <c r="E87" s="14"/>
       <c r="F87" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="88" spans="1:6" ht="14.25" customHeight="1">
@@ -2022,7 +2033,7 @@
       <c r="E88" s="14"/>
       <c r="F88" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="89" spans="1:6" ht="14.25" customHeight="1">
@@ -2033,7 +2044,7 @@
       <c r="E89" s="14"/>
       <c r="F89" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="14.25" customHeight="1">
@@ -2044,7 +2055,7 @@
       <c r="E90" s="14"/>
       <c r="F90" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="91" spans="1:6" ht="14.25" customHeight="1">
@@ -2055,7 +2066,7 @@
       <c r="E91" s="14"/>
       <c r="F91" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="92" spans="1:6" ht="14.25" customHeight="1">
@@ -2066,52 +2077,52 @@
       <c r="E92" s="14"/>
       <c r="F92" s="9">
         <f t="shared" si="0"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="93" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A93" s="24" t="s">
+      <c r="A93" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B93" s="25"/>
-      <c r="C93" s="26"/>
+      <c r="B93" s="27"/>
+      <c r="C93" s="28"/>
       <c r="D93" s="6">
         <f>SUM(D3:D92)</f>
-        <v>293330</v>
+        <v>643330</v>
       </c>
       <c r="E93" s="17"/>
       <c r="F93" s="9">
         <f t="shared" ref="F93:F94" si="1">F91</f>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A94" s="30" t="s">
+      <c r="A94" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B94" s="28"/>
-      <c r="C94" s="28"/>
-      <c r="D94" s="29"/>
+      <c r="B94" s="30"/>
+      <c r="C94" s="30"/>
+      <c r="D94" s="31"/>
       <c r="E94" s="18">
         <f>SUM(E11:E92)</f>
         <v>500000</v>
       </c>
       <c r="F94" s="9">
         <f t="shared" si="1"/>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="14.25" customHeight="1">
-      <c r="A95" s="31" t="s">
+      <c r="A95" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B95" s="32"/>
-      <c r="C95" s="32"/>
-      <c r="D95" s="32"/>
-      <c r="E95" s="33"/>
+      <c r="B95" s="34"/>
+      <c r="C95" s="34"/>
+      <c r="D95" s="34"/>
+      <c r="E95" s="35"/>
       <c r="F95" s="19">
         <f>F92</f>
-        <v>456670</v>
+        <v>106670</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Update cash book Excel files
Revised 'Cash Book for staff.xlsx' and 'Expenditure Mian Anjum Saeed.xlsx' with new data or corrections.
</commit_message>
<xml_diff>
--- a/Cash Book/Expenditure Mian Anjum Saeed.xlsx
+++ b/Cash Book/Expenditure Mian Anjum Saeed.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mian-Industries\Mian-Industries\Cash Book\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Mian-Industries\Cash Book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAE2E49-21C6-47E0-8CE1-9CE01B754A57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Up untill 2025" sheetId="1" r:id="rId1"/>
@@ -185,7 +184,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
@@ -781,20 +780,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="6" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.5546875" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" customWidth="1"/>
+    <col min="6" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.25" customHeight="1">

</xml_diff>